<commit_message>
resolve some constraint violations in sample data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acciopacus/Desktop/CS2102/cs2102-team61/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{08001DF8-A667-3541-BD9C-5B151734CB9B}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{12A566AD-827F-E146-8A96-DE610BC29D5D}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" firstSheet="11" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" firstSheet="11" activeTab="18" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="208">
   <si>
     <t>eid</t>
   </si>
@@ -411,9 +411,6 @@
   </si>
   <si>
     <t>Structure of Sentences and Meanings</t>
-  </si>
-  <si>
-    <t>English Language and Literature</t>
   </si>
   <si>
     <t>cid</t>
@@ -1700,7 +1697,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1784,7 +1781,7 @@
         <v>115</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>97</v>
@@ -1801,7 +1798,7 @@
         <v>116</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>99</v>
@@ -1818,7 +1815,7 @@
         <v>117</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>99</v>
@@ -1835,7 +1832,7 @@
         <v>118</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>101</v>
@@ -1852,7 +1849,7 @@
         <v>119</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>101</v>
@@ -1886,10 +1883,10 @@
         <v>122</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>123</v>
+        <v>102</v>
       </c>
       <c r="E11" s="3">
         <v>1</v>
@@ -1912,37 +1909,39 @@
   </sheetPr>
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>73</v>
       </c>
       <c r="H1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2040,7 +2039,7 @@
         <v>44265</v>
       </c>
       <c r="C5" s="2">
-        <v>44296</v>
+        <v>44295</v>
       </c>
       <c r="D5" s="2">
         <v>44301</v>
@@ -2098,7 +2097,7 @@
         <v>44265</v>
       </c>
       <c r="C7" s="2">
-        <v>44296</v>
+        <v>44295</v>
       </c>
       <c r="D7" s="2">
         <v>44301</v>
@@ -2162,7 +2161,7 @@
         <v>44230</v>
       </c>
       <c r="E9" s="2">
-        <v>43845</v>
+        <v>44211</v>
       </c>
       <c r="F9" s="1">
         <v>150</v>
@@ -2185,7 +2184,7 @@
         <v>44265</v>
       </c>
       <c r="C10" s="2">
-        <v>44296</v>
+        <v>44295</v>
       </c>
       <c r="D10" s="2">
         <v>44301</v>
@@ -2217,7 +2216,7 @@
         <v>44252</v>
       </c>
       <c r="D11" s="2">
-        <v>44255</v>
+        <v>44253</v>
       </c>
       <c r="E11" s="2">
         <v>44242</v>
@@ -2247,33 +2246,33 @@
   </sheetPr>
   <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+    <sheetView topLeftCell="A7" zoomScale="170" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>125</v>
-      </c>
       <c r="C1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>135</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>136</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>71</v>
@@ -2368,7 +2367,7 @@
         <v>2</v>
       </c>
       <c r="D5" s="2">
-        <v>44185</v>
+        <v>44183</v>
       </c>
       <c r="E5" s="1">
         <v>14</v>
@@ -2446,7 +2445,7 @@
         <v>1</v>
       </c>
       <c r="D8" s="9">
-        <v>44296</v>
+        <v>44295</v>
       </c>
       <c r="E8" s="8">
         <v>14</v>
@@ -2550,13 +2549,13 @@
         <v>1</v>
       </c>
       <c r="D12" s="9">
-        <v>44296</v>
+        <v>44295</v>
       </c>
       <c r="E12" s="8">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F12" s="8">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G12" s="8">
         <v>5</v>
@@ -2657,10 +2656,10 @@
         <v>44228</v>
       </c>
       <c r="E16" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F16" s="1">
-        <v>14.5</v>
+        <v>16.5</v>
       </c>
       <c r="G16" s="1">
         <v>12</v>
@@ -2683,10 +2682,10 @@
         <v>44230</v>
       </c>
       <c r="E17" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="F17" s="1">
-        <v>14.5</v>
+        <v>16.5</v>
       </c>
       <c r="G17" s="1">
         <v>12</v>
@@ -2706,7 +2705,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="9">
-        <v>44296</v>
+        <v>44295</v>
       </c>
       <c r="E18" s="8">
         <v>14</v>
@@ -2784,7 +2783,7 @@
         <v>2</v>
       </c>
       <c r="D21" s="2">
-        <v>44255</v>
+        <v>44253</v>
       </c>
       <c r="E21" s="1">
         <v>17</v>
@@ -2822,13 +2821,13 @@
   <sheetData>
     <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2900,7 +2899,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>15</v>
       </c>
@@ -2908,7 +2907,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>16</v>
       </c>
@@ -2934,7 +2933,7 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>94</v>
@@ -2954,16 +2953,16 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>140</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>141</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2971,16 +2970,16 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -2988,16 +2987,16 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="C4" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D4" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3005,16 +3004,16 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="D5" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="E5" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3022,16 +3021,16 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="D6" s="1" t="s">
-        <v>156</v>
-      </c>
       <c r="E6" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3039,16 +3038,16 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>159</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3056,16 +3055,16 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C8" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="D8" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="E8" s="1" t="s">
         <v>162</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3073,16 +3072,16 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="C9" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="D9" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="1" t="s">
         <v>166</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3090,16 +3089,16 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C10" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="D10" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>171</v>
       </c>
     </row>
     <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3107,16 +3106,16 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C11" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="D11" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="D11" s="1" t="s">
-        <v>174</v>
-      </c>
       <c r="E11" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>
@@ -3137,18 +3136,18 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>176</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B2" s="2">
         <v>45476</v>
@@ -3159,7 +3158,7 @@
     </row>
     <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3" s="2">
         <v>45477</v>
@@ -3170,7 +3169,7 @@
     </row>
     <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B4" s="2">
         <v>45478</v>
@@ -3181,7 +3180,7 @@
     </row>
     <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B5" s="2">
         <v>45479</v>
@@ -3192,7 +3191,7 @@
     </row>
     <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B6" s="2">
         <v>45480</v>
@@ -3203,7 +3202,7 @@
     </row>
     <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B7" s="2">
         <v>45481</v>
@@ -3214,7 +3213,7 @@
     </row>
     <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B8" s="2">
         <v>45482</v>
@@ -3225,7 +3224,7 @@
     </row>
     <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B9" s="2">
         <v>45483</v>
@@ -3236,7 +3235,7 @@
     </row>
     <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B10" s="2">
         <v>45484</v>
@@ -3247,7 +3246,7 @@
     </row>
     <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B11" s="2">
         <v>45485</v>
@@ -3274,13 +3273,13 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3288,7 +3287,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C2" s="2">
         <v>43649</v>
@@ -3299,7 +3298,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C3" s="2">
         <v>43650</v>
@@ -3310,7 +3309,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="C4" s="2">
         <v>43651</v>
@@ -3321,7 +3320,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="C5" s="2">
         <v>43652</v>
@@ -3332,7 +3331,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C6" s="2">
         <v>43653</v>
@@ -3343,7 +3342,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C7" s="2">
         <v>43654</v>
@@ -3354,7 +3353,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C8" s="2">
         <v>43655</v>
@@ -3365,7 +3364,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C9" s="2">
         <v>43656</v>
@@ -3376,7 +3375,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="C10" s="2">
         <v>43657</v>
@@ -3387,7 +3386,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C11" s="2">
         <v>43658</v>
@@ -3405,7 +3404,9 @@
   </sheetPr>
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="219" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3414,22 +3415,22 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>94</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3446,7 +3447,7 @@
         <v>42730</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="F2" s="1">
         <v>166</v>
@@ -3466,7 +3467,7 @@
         <v>46973</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="F3" s="1">
         <v>178</v>
@@ -3486,7 +3487,7 @@
         <v>47483</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="F4" s="1">
         <v>233</v>
@@ -3506,7 +3507,7 @@
         <v>44594</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="F5" s="1">
         <v>399</v>
@@ -3628,9 +3629,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="170" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
@@ -3639,16 +3642,16 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3656,7 +3659,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C2" s="2">
         <v>42528</v>
@@ -3670,7 +3673,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C3" s="2">
         <v>43320</v>
@@ -3684,7 +3687,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C4" s="2">
         <v>44581</v>
@@ -3698,7 +3701,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C5" s="2">
         <v>44593</v>
@@ -3712,13 +3715,24 @@
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="C6" s="2">
         <v>44594</v>
       </c>
       <c r="D6" s="1">
         <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>2</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C7" s="2">
+        <v>43321</v>
       </c>
     </row>
   </sheetData>
@@ -3733,39 +3747,41 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView zoomScale="194" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>104</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="C2" s="2">
         <v>43320</v>
@@ -3780,7 +3796,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="2">
-        <v>43322</v>
+        <v>44247</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3788,7 +3804,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C3" s="2">
         <v>43321</v>
@@ -3824,24 +3840,24 @@
   <sheetData>
     <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -3858,7 +3874,7 @@
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B3" s="1">
         <v>2</v>
@@ -3873,9 +3889,9 @@
         <v>44166</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B4" s="3">
         <v>3</v>
@@ -3902,7 +3918,7 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="168" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
@@ -3910,30 +3926,30 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>104</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>133</v>
-      </c>
       <c r="F1" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>201</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B2" s="1">
         <v>1</v>
@@ -3956,7 +3972,7 @@
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B3" s="1">
         <v>4</v>

</xml_diff>

<commit_message>
resolve manager constraint violations
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hello\Documents\GitHub\cs2102-team61\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acciopacus/Desktop/CS2102/cs2102-team61/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878EB1A2-0C89-445F-8B05-718968C54A00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{C71358F9-20BF-6D4B-B663-38849ED55B11}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="953" firstSheet="11" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="953" firstSheet="1" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -984,17 +984,17 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="L13" sqref="L13"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="3" max="3" width="17.6328125" customWidth="1"/>
-    <col min="4" max="4" width="22.6328125" customWidth="1"/>
-    <col min="5" max="5" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="17.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="5" max="5" width="20.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1017,7 +1017,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1037,7 +1037,7 @@
         <v>42008</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1060,7 +1060,7 @@
         <v>43805</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>42976</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1100,7 +1100,7 @@
         <v>42372</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1120,7 +1120,7 @@
         <v>39451</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1137,7 +1137,7 @@
         <v>43470</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1160,7 +1160,7 @@
         <v>44260</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1181,7 +1181,7 @@
       </c>
       <c r="G9" s="2"/>
     </row>
-    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1198,7 +1198,7 @@
         <v>43838</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1219,7 +1219,7 @@
       </c>
       <c r="G11" s="2"/>
     </row>
-    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1240,7 +1240,7 @@
       </c>
       <c r="G12" s="2"/>
     </row>
-    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1260,7 +1260,7 @@
         <v>44085</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>44262</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1303,7 +1303,7 @@
         <v>44283</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1323,7 +1323,7 @@
         <v>43538</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1357,12 +1357,12 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="43.453125" customWidth="1"/>
+    <col min="2" max="2" width="43.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>71</v>
       </c>
@@ -1373,7 +1373,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1384,7 +1384,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1395,7 +1395,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1406,7 +1406,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1428,7 +1428,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1439,7 +1439,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1450,7 +1450,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1461,7 +1461,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1472,7 +1472,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1483,7 +1483,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1494,7 +1494,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1505,7 +1505,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1516,7 +1516,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1527,7 +1527,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -1549,7 +1549,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -1560,7 +1560,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -1571,7 +1571,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -1605,14 +1605,16 @@
   </sheetPr>
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>94</v>
       </c>
@@ -1620,7 +1622,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>96</v>
       </c>
@@ -1628,7 +1630,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>97</v>
       </c>
@@ -1636,7 +1638,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="5" t="s">
         <v>98</v>
       </c>
@@ -1644,31 +1646,31 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="5" t="s">
         <v>99</v>
       </c>
       <c r="B5" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="5" t="s">
         <v>100</v>
       </c>
       <c r="B6" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="5" t="s">
         <v>101</v>
       </c>
       <c r="B7" s="4">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="5" t="s">
         <v>102</v>
       </c>
@@ -1676,7 +1678,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="5" t="s">
         <v>103</v>
       </c>
@@ -1700,12 +1702,12 @@
       <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="26.1796875" customWidth="1"/>
+    <col min="2" max="2" width="26.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>104</v>
       </c>
@@ -1722,7 +1724,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3">
         <v>1</v>
       </c>
@@ -1739,7 +1741,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3">
         <v>2</v>
       </c>
@@ -1756,7 +1758,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -1773,7 +1775,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -1790,7 +1792,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3">
         <v>5</v>
       </c>
@@ -1807,7 +1809,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3">
         <v>6</v>
       </c>
@@ -1824,7 +1826,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>7</v>
       </c>
@@ -1841,7 +1843,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>8</v>
       </c>
@@ -1858,7 +1860,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>9</v>
       </c>
@@ -1875,7 +1877,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>10</v>
       </c>
@@ -1913,9 +1915,9 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>123</v>
       </c>
@@ -1944,7 +1946,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1973,7 +1975,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2002,7 +2004,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2031,7 +2033,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -2060,7 +2062,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -2089,7 +2091,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>4</v>
       </c>
@@ -2118,7 +2120,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>5</v>
       </c>
@@ -2147,7 +2149,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>5</v>
       </c>
@@ -2176,7 +2178,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -2205,7 +2207,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -2250,9 +2252,9 @@
       <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>123</v>
       </c>
@@ -2278,7 +2280,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2304,7 +2306,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -2330,7 +2332,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -2356,7 +2358,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>2</v>
       </c>
@@ -2382,7 +2384,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>2</v>
       </c>
@@ -2408,7 +2410,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -2434,7 +2436,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="8">
         <v>3</v>
       </c>
@@ -2460,7 +2462,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="11">
         <v>3</v>
       </c>
@@ -2486,7 +2488,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>4</v>
       </c>
@@ -2512,7 +2514,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>4</v>
       </c>
@@ -2538,7 +2540,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A12" s="8">
         <v>4</v>
       </c>
@@ -2564,7 +2566,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A13" s="11">
         <v>4</v>
       </c>
@@ -2590,7 +2592,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A14" s="1">
         <v>5</v>
       </c>
@@ -2616,7 +2618,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A15" s="1">
         <v>5</v>
       </c>
@@ -2642,7 +2644,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A16" s="1">
         <v>5</v>
       </c>
@@ -2668,7 +2670,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A17" s="1">
         <v>5</v>
       </c>
@@ -2694,7 +2696,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A18" s="8">
         <v>5</v>
       </c>
@@ -2720,7 +2722,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A19" s="11">
         <v>5</v>
       </c>
@@ -2746,7 +2748,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A20" s="1">
         <v>6</v>
       </c>
@@ -2772,7 +2774,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="12.5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:8" ht="13" x14ac:dyDescent="0.15">
       <c r="A21" s="1">
         <v>6</v>
       </c>
@@ -2814,12 +2816,12 @@
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="2" max="2" width="23.1796875" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>135</v>
       </c>
@@ -2827,7 +2829,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2835,7 +2837,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2843,7 +2845,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2851,7 +2853,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -2859,7 +2861,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -2867,7 +2869,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>11</v>
       </c>
@@ -2875,7 +2877,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>12</v>
       </c>
@@ -2883,7 +2885,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>13</v>
       </c>
@@ -2891,7 +2893,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>14</v>
       </c>
@@ -2899,7 +2901,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>15</v>
       </c>
@@ -2907,7 +2909,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>16</v>
       </c>
@@ -2929,9 +2931,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>123</v>
       </c>
@@ -2948,7 +2950,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -2965,7 +2967,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -2982,7 +2984,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -2999,7 +3001,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3016,7 +3018,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3033,7 +3035,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3050,7 +3052,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3067,7 +3069,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3084,7 +3086,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3101,7 +3103,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3134,9 +3136,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>174</v>
       </c>
@@ -3147,7 +3149,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>177</v>
       </c>
@@ -3158,7 +3160,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>178</v>
       </c>
@@ -3169,7 +3171,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>179</v>
       </c>
@@ -3180,7 +3182,7 @@
         <v>788</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1" t="s">
         <v>180</v>
       </c>
@@ -3191,7 +3193,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1" t="s">
         <v>181</v>
       </c>
@@ -3202,7 +3204,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1" t="s">
         <v>182</v>
       </c>
@@ -3213,7 +3215,7 @@
         <v>777</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1" t="s">
         <v>183</v>
       </c>
@@ -3224,7 +3226,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1" t="s">
         <v>184</v>
       </c>
@@ -3235,7 +3237,7 @@
         <v>999</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1" t="s">
         <v>185</v>
       </c>
@@ -3246,7 +3248,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1" t="s">
         <v>186</v>
       </c>
@@ -3273,9 +3275,9 @@
       <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>123</v>
       </c>
@@ -3286,7 +3288,7 @@
         <v>187</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3297,7 +3299,7 @@
         <v>43649</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3308,7 +3310,7 @@
         <v>43650</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3319,7 +3321,7 @@
         <v>43651</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3330,7 +3332,7 @@
         <v>43652</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3341,7 +3343,7 @@
         <v>43653</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3352,7 +3354,7 @@
         <v>43654</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3363,7 +3365,7 @@
         <v>43655</v>
       </c>
     </row>
-    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3374,7 +3376,7 @@
         <v>43656</v>
       </c>
     </row>
-    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3385,7 +3387,7 @@
         <v>43657</v>
       </c>
     </row>
-    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3412,12 +3414,12 @@
       <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="5" max="5" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>188</v>
       </c>
@@ -3437,7 +3439,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3457,7 +3459,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3477,7 +3479,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3497,7 +3499,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3533,9 +3535,9 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3543,7 +3545,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3551,7 +3553,7 @@
         <v>10000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3559,7 +3561,7 @@
         <v>9000</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3567,7 +3569,7 @@
         <v>8888</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -3575,7 +3577,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -3583,7 +3585,7 @@
         <v>5000</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -3591,7 +3593,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -3599,7 +3601,7 @@
         <v>123456</v>
       </c>
     </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -3607,7 +3609,7 @@
         <v>987</v>
       </c>
     </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -3615,7 +3617,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -3639,12 +3641,12 @@
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="4" max="4" width="23.453125" customWidth="1"/>
+    <col min="4" max="4" width="23.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>188</v>
       </c>
@@ -3658,7 +3660,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3672,7 +3674,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3686,7 +3688,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -3700,7 +3702,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -3714,7 +3716,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>3</v>
       </c>
@@ -3728,7 +3730,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -3755,12 +3757,12 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView zoomScale="133" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>188</v>
       </c>
@@ -3783,7 +3785,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>2</v>
       </c>
@@ -3806,7 +3808,7 @@
         <v>44247</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -3845,9 +3847,9 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>174</v>
       </c>
@@ -3864,7 +3866,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1" t="s">
         <v>177</v>
       </c>
@@ -3881,7 +3883,7 @@
         <v>44096</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1" t="s">
         <v>178</v>
       </c>
@@ -3898,7 +3900,7 @@
         <v>44166</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="15.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>186</v>
       </c>
@@ -3927,13 +3929,13 @@
   </sheetPr>
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+    <sheetView zoomScale="107" workbookViewId="0">
       <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>199</v>
       </c>
@@ -3956,7 +3958,7 @@
         <v>201</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -3979,7 +3981,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>5</v>
       </c>
@@ -4018,9 +4020,9 @@
       <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4028,7 +4030,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>11</v>
       </c>
@@ -4036,7 +4038,7 @@
         <v>2000</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>12</v>
       </c>
@@ -4044,7 +4046,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>13</v>
       </c>
@@ -4052,7 +4054,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>14</v>
       </c>
@@ -4060,7 +4062,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>15</v>
       </c>
@@ -4068,7 +4070,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>16</v>
       </c>
@@ -4090,64 +4092,64 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A10" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A11" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="1">
         <v>16</v>
       </c>
@@ -4166,34 +4168,34 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -4212,39 +4214,39 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="1">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="1">
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="1">
         <v>16</v>
       </c>
@@ -4263,19 +4265,19 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>10</v>
       </c>
@@ -4294,24 +4296,24 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="1">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="1">
         <v>8</v>
       </c>
@@ -4330,9 +4332,9 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
Added more test data for package sales. Cleaned Buys data for num_remaining_redemptions to match with redeems and cancels record. Finished testing on Q27.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/cs2102-team61/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2636361-E134-6F40-8A01-1F89281C8292}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815C332D-1EC9-A949-8AA6-82764E2F7981}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2480" yWindow="840" windowWidth="25600" windowHeight="16000" tabRatio="953" firstSheet="11" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="820" windowWidth="25600" windowHeight="16000" tabRatio="953" firstSheet="11" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="314" uniqueCount="211">
   <si>
     <t>eid</t>
   </si>
@@ -666,6 +666,15 @@
   </si>
   <si>
     <t xml:space="preserve">This module explores language structure, in particular, patterns of sentence structure (syntax) and of meaning (semantics) in English. </t>
+  </si>
+  <si>
+    <t>HAPPY NEW YEAR</t>
+  </si>
+  <si>
+    <t>HAPPY NEW MONTH</t>
+  </si>
+  <si>
+    <t>HAPPY APRIL FOOLS</t>
   </si>
 </sst>
 </file>
@@ -2404,7 +2413,7 @@
   <dimension ref="A1:H28"/>
   <sheetViews>
     <sheetView zoomScale="118" workbookViewId="0">
-      <selection activeCell="A27" sqref="A27:D27"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3470,7 +3479,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView zoomScale="118" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3609,7 +3618,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3745,10 +3754,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView zoomScale="73" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3833,7 +3842,7 @@
         <v>195</v>
       </c>
       <c r="F4" s="1">
-        <v>233</v>
+        <v>308</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3854,6 +3863,66 @@
       </c>
       <c r="F5" s="1">
         <v>399</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1">
+        <v>10</v>
+      </c>
+      <c r="C6" s="2">
+        <v>44228</v>
+      </c>
+      <c r="D6" s="2">
+        <v>44531</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="F6" s="1">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1">
+        <v>10</v>
+      </c>
+      <c r="C7" s="2">
+        <v>44256</v>
+      </c>
+      <c r="D7" s="2">
+        <v>44532</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="F7" s="1">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1">
+        <v>15</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44287</v>
+      </c>
+      <c r="D8" s="2">
+        <v>44533</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="F8" s="1">
+        <v>233</v>
       </c>
     </row>
   </sheetData>
@@ -3972,10 +4041,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView zoomScale="127" workbookViewId="0">
-      <selection activeCell="C2" activeCellId="1" sqref="B2 C2"/>
+    <sheetView tabSelected="1" zoomScale="127" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4008,7 +4077,7 @@
         <v>42528</v>
       </c>
       <c r="D2" s="1">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4022,7 +4091,7 @@
         <v>43381</v>
       </c>
       <c r="D3" s="7">
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4064,7 +4133,7 @@
         <v>44197</v>
       </c>
       <c r="D6" s="1">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4079,6 +4148,62 @@
       </c>
       <c r="D7" s="1">
         <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A8" s="1">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C8" s="2">
+        <v>44288</v>
+      </c>
+      <c r="D8" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A9" s="1">
+        <v>5</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" s="2">
+        <v>44288</v>
+      </c>
+      <c r="D9" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A10" s="1">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C10" s="2">
+        <v>44288</v>
+      </c>
+      <c r="D10" s="1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A11" s="1">
+        <v>7</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="C11" s="2">
+        <v>44288</v>
+      </c>
+      <c r="D11" s="1">
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -4094,7 +4219,7 @@
   <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView zoomScale="133" zoomScaleNormal="133" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4507,7 +4632,7 @@
   </sheetPr>
   <dimension ref="A1:G4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="107" workbookViewId="0">
+    <sheetView zoomScale="107" workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Update data to pass new triggers
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/cs2102-team61/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenzaza/Desktop/cs2103-projects/cs2102-team61/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{815C332D-1EC9-A949-8AA6-82764E2F7981}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED5E99D-E0B3-B84B-8E6C-58536B9CA972}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2460" yWindow="820" windowWidth="25600" windowHeight="16000" tabRatio="953" firstSheet="11" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2460" yWindow="780" windowWidth="25600" windowHeight="16000" tabRatio="953" firstSheet="11" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -727,7 +727,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -746,6 +746,12 @@
         <bgColor rgb="FF93C47D"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -759,7 +765,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -780,6 +786,9 @@
     <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="1" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1931,7 +1940,7 @@
   <dimension ref="A1:I16"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3618,7 +3627,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4044,7 +4053,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="127" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4091,7 +4100,7 @@
         <v>43381</v>
       </c>
       <c r="D3" s="7">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4267,29 +4276,29 @@
         <v>1</v>
       </c>
       <c r="G2" s="2">
-        <v>44247</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="1">
+        <v>44242</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" s="20" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="18">
         <v>2</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3" s="19">
         <v>43381</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" s="18">
         <v>4</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3" s="19">
         <v>44075</v>
       </c>
-      <c r="F3" s="1">
-        <v>1</v>
-      </c>
-      <c r="G3" s="2">
+      <c r="F3" s="18">
+        <v>1</v>
+      </c>
+      <c r="G3" s="19">
         <v>44084</v>
       </c>
     </row>
@@ -4313,7 +4322,7 @@
         <v>1</v>
       </c>
       <c r="G4" s="2">
-        <v>44228</v>
+        <v>44197</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4336,7 +4345,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="9">
-        <v>44295</v>
+        <v>44285</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4352,14 +4361,14 @@
       <c r="D6" s="1">
         <v>5</v>
       </c>
-      <c r="E6" s="16">
-        <v>44285</v>
+      <c r="E6" s="2">
+        <v>44265</v>
       </c>
       <c r="F6" s="1">
         <v>1</v>
       </c>
       <c r="G6" s="2">
-        <v>44326</v>
+        <v>44265</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4382,7 +4391,7 @@
         <v>1</v>
       </c>
       <c r="G7" s="2">
-        <v>44228</v>
+        <v>44216</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4405,7 +4414,7 @@
         <v>2</v>
       </c>
       <c r="G8" s="2">
-        <v>44256</v>
+        <v>44245</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4428,7 +4437,7 @@
         <v>3</v>
       </c>
       <c r="G9" s="2">
-        <v>44287</v>
+        <v>44273</v>
       </c>
     </row>
   </sheetData>
@@ -4445,7 +4454,7 @@
   <dimension ref="A1:E10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4481,7 +4490,7 @@
         <v>2</v>
       </c>
       <c r="E2" s="14">
-        <v>44096</v>
+        <v>44094</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4498,7 +4507,7 @@
         <v>1</v>
       </c>
       <c r="E3" s="2">
-        <v>44166</v>
+        <v>44136</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="16" x14ac:dyDescent="0.2">
@@ -4515,7 +4524,7 @@
         <v>1</v>
       </c>
       <c r="E4" s="15">
-        <v>44294</v>
+        <v>44273</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4532,7 +4541,7 @@
         <v>2</v>
       </c>
       <c r="E5" s="12">
-        <v>44301</v>
+        <v>44270</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4549,7 +4558,7 @@
         <v>1</v>
       </c>
       <c r="E6" s="2">
-        <v>44326</v>
+        <v>44296</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4566,7 +4575,7 @@
         <v>1</v>
       </c>
       <c r="E7" s="2">
-        <v>44326</v>
+        <v>44297</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4583,7 +4592,7 @@
         <v>2</v>
       </c>
       <c r="E8" s="2">
-        <v>44256</v>
+        <v>44229</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4600,7 +4609,7 @@
         <v>3</v>
       </c>
       <c r="E9" s="2">
-        <v>44287</v>
+        <v>44258</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -4617,7 +4626,7 @@
         <v>3</v>
       </c>
       <c r="E10" s="2">
-        <v>44287</v>
+        <v>44258</v>
       </c>
     </row>
   </sheetData>
@@ -4633,7 +4642,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView zoomScale="107" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>

</xml_diff>

<commit_message>
Change data for Sessions
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10709"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/acciopacus/Desktop/CS2102/cs2102-team61/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenzaza/Desktop/cs2103-projects/cs2102-team61/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{E2EAADB1-C256-0D49-8AA5-3270E169551F}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80507B29-A40C-3C4F-8374-089D77A71B88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" firstSheet="11" activeTab="19" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15540" firstSheet="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -24,10 +24,10 @@
     <sheet name="Pay_slips" sheetId="9" r:id="rId9"/>
     <sheet name="Rooms" sheetId="10" r:id="rId10"/>
     <sheet name="Course_areas" sheetId="11" r:id="rId11"/>
-    <sheet name="Courses" sheetId="12" r:id="rId12"/>
-    <sheet name="Offerings" sheetId="13" r:id="rId13"/>
-    <sheet name="Sessions" sheetId="14" r:id="rId14"/>
-    <sheet name="Specializes" sheetId="15" r:id="rId15"/>
+    <sheet name="Specializes" sheetId="15" r:id="rId12"/>
+    <sheet name="Courses" sheetId="12" r:id="rId13"/>
+    <sheet name="Offerings" sheetId="13" r:id="rId14"/>
+    <sheet name="Sessions" sheetId="14" r:id="rId15"/>
     <sheet name="Customers" sheetId="16" r:id="rId16"/>
     <sheet name="Credit_cards" sheetId="17" r:id="rId17"/>
     <sheet name="Owns" sheetId="18" r:id="rId18"/>
@@ -1245,8 +1245,8 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -1322,7 +1322,7 @@
         <v>43101</v>
       </c>
       <c r="G3" s="3">
-        <v>43805</v>
+        <v>44292</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1">
@@ -2081,6 +2081,142 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
+  <sheetPr>
+    <outlinePr summaryBelow="0" summaryRight="0"/>
+  </sheetPr>
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
+  <cols>
+    <col min="1" max="1" width="14.5" customWidth="1"/>
+    <col min="2" max="2" width="23.1640625" customWidth="1"/>
+    <col min="3" max="6" width="14.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="10" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A7" s="1">
+        <v>11</v>
+      </c>
+      <c r="B7" s="10" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A8" s="1">
+        <v>12</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A9" s="1">
+        <v>13</v>
+      </c>
+      <c r="B9" s="10" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A10" s="1">
+        <v>14</v>
+      </c>
+      <c r="B10" s="10" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A11" s="1">
+        <v>15</v>
+      </c>
+      <c r="B11" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A12" s="1">
+        <v>16</v>
+      </c>
+      <c r="B12" s="10" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A13" s="4">
+        <v>17</v>
+      </c>
+      <c r="B13" s="10" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" ht="15.75" customHeight="1">
+      <c r="A14" s="4">
+        <v>20</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>116</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
+  <pageSetup orientation="landscape"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2293,7 +2429,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
@@ -2837,15 +2973,15 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0D00-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -3865,142 +4001,6 @@
       </c>
       <c r="H39" s="4">
         <v>21</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="landscape"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0E00-000000000000}">
-  <sheetPr>
-    <outlinePr summaryBelow="0" summaryRight="0"/>
-  </sheetPr>
-  <dimension ref="A1:B14"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
-  <cols>
-    <col min="1" max="1" width="14.5" customWidth="1"/>
-    <col min="2" max="2" width="23.1640625" customWidth="1"/>
-    <col min="3" max="6" width="14.5" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A1" s="1" t="s">
-        <v>162</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="8" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A3" s="1">
-        <v>2</v>
-      </c>
-      <c r="B3" s="10" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A4" s="1">
-        <v>3</v>
-      </c>
-      <c r="B4" s="10" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A5" s="1">
-        <v>4</v>
-      </c>
-      <c r="B5" s="10" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A6" s="1">
-        <v>5</v>
-      </c>
-      <c r="B6" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A7" s="1">
-        <v>11</v>
-      </c>
-      <c r="B7" s="10" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A8" s="1">
-        <v>12</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A9" s="1">
-        <v>13</v>
-      </c>
-      <c r="B9" s="10" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A10" s="1">
-        <v>14</v>
-      </c>
-      <c r="B10" s="10" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A11" s="1">
-        <v>15</v>
-      </c>
-      <c r="B11" s="10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A12" s="1">
-        <v>16</v>
-      </c>
-      <c r="B12" s="10" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A13" s="4">
-        <v>17</v>
-      </c>
-      <c r="B13" s="10" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="15.75" customHeight="1">
-      <c r="A14" s="4">
-        <v>20</v>
-      </c>
-      <c r="B14" s="8" t="s">
-        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -5424,7 +5424,7 @@
   </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed bugs in data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10713"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chenzaza/Desktop/cs2103-projects/cs2102-team61/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/cs2102-team61/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80507B29-A40C-3C4F-8374-089D77A71B88}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C7F7B27-1B76-554E-9C4F-C1B20EC681B5}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="15540" firstSheet="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="480" windowWidth="25600" windowHeight="15540" firstSheet="6" activeTab="14" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -939,7 +939,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -964,6 +964,12 @@
         <bgColor rgb="FF93C47D"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -984,7 +990,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1025,6 +1031,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1245,8 +1259,8 @@
   </sheetPr>
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2088,7 +2102,7 @@
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD1048576"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2224,7 +2238,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2980,8 +2994,8 @@
   </sheetPr>
   <dimension ref="A1:H39"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M24" sqref="M24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -3139,7 +3153,7 @@
         <v>16</v>
       </c>
       <c r="G6" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H6" s="1">
         <v>8</v>
@@ -3165,7 +3179,7 @@
         <v>16</v>
       </c>
       <c r="G7" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H7" s="1">
         <v>8</v>
@@ -3191,7 +3205,7 @@
         <v>17</v>
       </c>
       <c r="G8" s="17">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="H8" s="17">
         <v>3</v>
@@ -3217,7 +3231,7 @@
         <v>17</v>
       </c>
       <c r="G9" s="19">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="H9" s="19">
         <v>3</v>
@@ -3243,7 +3257,7 @@
         <v>17</v>
       </c>
       <c r="G10" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="H10" s="1">
         <v>16</v>
@@ -3295,7 +3309,7 @@
         <v>17</v>
       </c>
       <c r="G12" s="17">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H12" s="17">
         <v>16</v>
@@ -3347,7 +3361,7 @@
         <v>10.5</v>
       </c>
       <c r="G14" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H14" s="1">
         <v>20</v>
@@ -3373,7 +3387,7 @@
         <v>11.5</v>
       </c>
       <c r="G15" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H15" s="1">
         <v>19</v>
@@ -3399,7 +3413,7 @@
         <v>16.5</v>
       </c>
       <c r="G16" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H16" s="1">
         <v>20</v>
@@ -3425,7 +3439,7 @@
         <v>16.5</v>
       </c>
       <c r="G17" s="1">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="H17" s="1">
         <v>19</v>
@@ -3451,7 +3465,7 @@
         <v>15.5</v>
       </c>
       <c r="G18" s="17">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H18" s="17">
         <v>20</v>
@@ -3477,7 +3491,7 @@
         <v>17</v>
       </c>
       <c r="G19" s="19">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H19" s="19">
         <v>18</v>
@@ -3503,7 +3517,7 @@
         <v>10</v>
       </c>
       <c r="G20" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H20" s="1">
         <v>20</v>
@@ -3529,7 +3543,7 @@
         <v>18</v>
       </c>
       <c r="G21" s="1">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="H21" s="1">
         <v>19</v>
@@ -3555,7 +3569,7 @@
         <v>16</v>
       </c>
       <c r="G22" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H22" s="1">
         <v>7</v>
@@ -3581,7 +3595,7 @@
         <v>12</v>
       </c>
       <c r="G23" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H23" s="1">
         <v>7</v>
@@ -3607,7 +3621,7 @@
         <v>18</v>
       </c>
       <c r="G24" s="1">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H24" s="1">
         <v>7</v>
@@ -3633,7 +3647,7 @@
         <v>15</v>
       </c>
       <c r="G25" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H25" s="1">
         <v>4</v>
@@ -3659,7 +3673,7 @@
         <v>15</v>
       </c>
       <c r="G26" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H26" s="1">
         <v>4</v>
@@ -3685,7 +3699,7 @@
         <v>15</v>
       </c>
       <c r="G27" s="1">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H27" s="1">
         <v>4</v>
@@ -3711,7 +3725,7 @@
         <v>10.5</v>
       </c>
       <c r="G28" s="1">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="H28" s="1">
         <v>15</v>
@@ -3737,7 +3751,7 @@
         <v>17</v>
       </c>
       <c r="G29" s="1">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="H29" s="1">
         <v>15</v>
@@ -3848,28 +3862,28 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A34" s="21">
+      <c r="A34" s="28">
         <v>10</v>
       </c>
-      <c r="B34" s="22">
+      <c r="B34" s="29">
         <v>44256</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="30">
         <v>5</v>
       </c>
-      <c r="D34" s="5">
+      <c r="D34" s="31">
         <v>44295</v>
       </c>
-      <c r="E34" s="4">
+      <c r="E34" s="30">
         <v>14</v>
       </c>
-      <c r="F34" s="4">
+      <c r="F34" s="30">
         <v>18</v>
       </c>
-      <c r="G34" s="4">
+      <c r="G34" s="30">
         <v>15</v>
       </c>
-      <c r="H34" s="4">
+      <c r="H34" s="30">
         <v>21</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified data. Fixed bug in Q19.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/cs2102-team61/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DDEC4873-C4D4-014E-AC15-65E72874D9CA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2BDBEA-26B1-E045-AB34-2A304903246E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="9" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="9" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -37,8 +37,17 @@
     <sheet name="Registers" sheetId="22" r:id="rId22"/>
     <sheet name="Cancels" sheetId="23" r:id="rId23"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext uri="GoogleSheetsCustomDataVersion1">
       <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId27" roundtripDataSignature="AMtx7mhKG3Zlx72GLTVwlsHN/7s2RNYUJw=="/>
     </ext>
@@ -47,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="430" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="280">
   <si>
     <t>eid</t>
   </si>
@@ -1260,7 +1269,7 @@
   <dimension ref="A1:G21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2451,7 +2460,7 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="H18" sqref="H18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -3024,7 +3033,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -4846,7 +4855,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -5494,7 +5503,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -5702,7 +5711,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A11" sqref="A11:XFD11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -5976,10 +5985,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="L26" sqref="L26"/>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="A13" sqref="A13:E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -6189,6 +6198,23 @@
       </c>
       <c r="E12" s="3">
         <v>44258</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15" customHeight="1">
+      <c r="A13" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="B13" s="2">
+        <v>10</v>
+      </c>
+      <c r="C13" s="14">
+        <v>44256</v>
+      </c>
+      <c r="D13" s="2">
+        <v>8</v>
+      </c>
+      <c r="E13" s="14">
+        <v>44256</v>
       </c>
     </row>
   </sheetData>
@@ -6202,10 +6228,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:XFD4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -6302,6 +6328,30 @@
         <v>0</v>
       </c>
       <c r="G4" s="26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="15" customHeight="1">
+      <c r="A5" s="26">
+        <v>21</v>
+      </c>
+      <c r="B5" s="26">
+        <v>10</v>
+      </c>
+      <c r="C5" s="27">
+        <v>44256</v>
+      </c>
+      <c r="D5" s="26">
+        <v>8</v>
+      </c>
+      <c r="E5" s="27">
+        <v>44257</v>
+      </c>
+      <c r="F5">
+        <f>79.9*0.9</f>
+        <v>71.910000000000011</v>
+      </c>
+      <c r="G5" s="26">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Modified data. Modified Q22.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/cs2102-team61/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D2BDBEA-26B1-E045-AB34-2A304903246E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CA4685-B498-424A-9B31-7E669E416412}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="9" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="281">
   <si>
     <t>eid</t>
   </si>
@@ -896,6 +896,9 @@
   </si>
   <si>
     <t>pkg_credit</t>
+  </si>
+  <si>
+    <t>03-02</t>
   </si>
 </sst>
 </file>
@@ -1731,10 +1734,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:C22"/>
+  <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -1983,6 +1986,17 @@
         <v>113</v>
       </c>
       <c r="C22" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="15" customHeight="1">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="6" t="s">
+        <v>280</v>
+      </c>
+      <c r="C23" s="2">
         <v>1</v>
       </c>
     </row>
@@ -3033,7 +3047,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -4855,7 +4869,7 @@
   <dimension ref="A1:C26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -5502,8 +5516,8 @@
   </sheetPr>
   <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -5711,7 +5725,7 @@
   <dimension ref="A1:G11"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -5988,7 +6002,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:E13"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -6230,8 +6244,8 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Added data for cancel
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/cs2102-team61/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A0CA4685-B498-424A-9B31-7E669E416412}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{689F7F1A-5DA7-8C44-A831-D34972273953}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="9" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="9" activeTab="20" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="432" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="281">
   <si>
     <t>eid</t>
   </si>
@@ -1002,7 +1002,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1051,6 +1051,14 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1736,7 +1744,7 @@
   </sheetPr>
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+    <sheetView topLeftCell="A6" workbookViewId="0">
       <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
@@ -3047,7 +3055,7 @@
   <dimension ref="A1:H40"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A34" sqref="A34:D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -3888,54 +3896,54 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A33" s="21">
+      <c r="A33" s="28">
         <v>10</v>
       </c>
-      <c r="B33" s="22">
+      <c r="B33" s="29">
         <v>44256</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="30">
         <v>4</v>
       </c>
-      <c r="D33" s="5">
-        <v>44294</v>
-      </c>
-      <c r="E33" s="4">
+      <c r="D33" s="31">
+        <v>44295</v>
+      </c>
+      <c r="E33" s="30">
         <v>14</v>
       </c>
-      <c r="F33" s="4">
+      <c r="F33" s="30">
         <v>18</v>
       </c>
-      <c r="G33" s="4">
+      <c r="G33" s="30">
         <v>15</v>
       </c>
-      <c r="H33" s="4">
+      <c r="H33" s="30">
         <v>21</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="15.75" customHeight="1">
-      <c r="A34" s="28">
+      <c r="A34" s="32">
         <v>10</v>
       </c>
-      <c r="B34" s="29">
+      <c r="B34" s="33">
         <v>44256</v>
       </c>
-      <c r="C34" s="30">
+      <c r="C34" s="34">
         <v>5</v>
       </c>
-      <c r="D34" s="31">
-        <v>44295</v>
-      </c>
-      <c r="E34" s="30">
+      <c r="D34" s="35">
+        <v>44301</v>
+      </c>
+      <c r="E34" s="34">
         <v>14</v>
       </c>
-      <c r="F34" s="30">
+      <c r="F34" s="34">
         <v>18</v>
       </c>
-      <c r="G34" s="30">
+      <c r="G34" s="34">
         <v>15</v>
       </c>
-      <c r="H34" s="30">
+      <c r="H34" s="34">
         <v>21</v>
       </c>
     </row>
@@ -5517,7 +5525,7 @@
   <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="A3" sqref="A3:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -5722,10 +5730,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -5986,6 +5994,29 @@
       </c>
       <c r="G11" s="5">
         <v>44266</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="15" customHeight="1">
+      <c r="A12" s="26">
+        <v>2</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>240</v>
+      </c>
+      <c r="C12" s="27">
+        <v>43381</v>
+      </c>
+      <c r="D12" s="32">
+        <v>10</v>
+      </c>
+      <c r="E12" s="33">
+        <v>44256</v>
+      </c>
+      <c r="F12" s="34">
+        <v>5</v>
+      </c>
+      <c r="G12" s="33">
+        <v>44256</v>
       </c>
     </row>
   </sheetData>
@@ -6002,7 +6033,7 @@
   <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>

</xml_diff>

<commit_message>
Added data for Q30 testing
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/cs2102-team61/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E367423-E25C-8A4D-9A17-CDEE989D5C00}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{884D9AD9-E379-5943-8280-E7C64B34E6BE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="9" activeTab="13" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="9" activeTab="21" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="433" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="283">
   <si>
     <t>eid</t>
   </si>
@@ -899,6 +899,12 @@
   </si>
   <si>
     <t>03-02</t>
+  </si>
+  <si>
+    <t>Introduction to AI</t>
+  </si>
+  <si>
+    <t>easy AI module</t>
   </si>
 </sst>
 </file>
@@ -1002,7 +1008,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1059,6 +1065,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1745,7 +1752,7 @@
   <dimension ref="A1:C23"/>
   <sheetViews>
     <sheetView topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2266,10 +2273,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2468,6 +2475,23 @@
         <v>4</v>
       </c>
     </row>
+    <row r="12" spans="1:5" ht="15" customHeight="1">
+      <c r="A12" s="7">
+        <v>11</v>
+      </c>
+      <c r="B12" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>282</v>
+      </c>
+      <c r="D12" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="E12" s="7">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
@@ -2479,10 +2503,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:I19"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A20" sqref="A20:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -3039,6 +3063,35 @@
       </c>
       <c r="I19" s="2">
         <v>18</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" customHeight="1">
+      <c r="A20" s="2">
+        <v>11</v>
+      </c>
+      <c r="B20" s="36">
+        <v>44317</v>
+      </c>
+      <c r="C20" s="36">
+        <v>44348</v>
+      </c>
+      <c r="D20" s="36">
+        <v>44348</v>
+      </c>
+      <c r="E20" s="36">
+        <v>44321</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="2">
+        <v>1</v>
+      </c>
+      <c r="H20" s="2">
+        <v>59.9</v>
+      </c>
+      <c r="I20" s="2">
+        <v>9</v>
       </c>
     </row>
   </sheetData>
@@ -3052,10 +3105,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:H40"/>
+  <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F40" sqref="F40"/>
+      <selection activeCell="H41" sqref="H41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -4101,6 +4154,32 @@
       </c>
       <c r="H40" s="1">
         <v>15</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" ht="15" customHeight="1">
+      <c r="A41" s="2">
+        <v>11</v>
+      </c>
+      <c r="B41" s="36">
+        <v>44317</v>
+      </c>
+      <c r="C41" s="2">
+        <v>1</v>
+      </c>
+      <c r="D41" s="36">
+        <v>44348</v>
+      </c>
+      <c r="E41" s="2">
+        <v>14</v>
+      </c>
+      <c r="F41" s="2">
+        <v>17</v>
+      </c>
+      <c r="G41" s="2">
+        <v>3</v>
+      </c>
+      <c r="H41" s="2">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -5733,7 +5812,7 @@
   <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView zoomScale="117" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -6030,10 +6109,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E13"/>
+  <dimension ref="A1:E14"/>
   <sheetViews>
-    <sheetView zoomScale="125" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -6260,6 +6339,23 @@
       </c>
       <c r="E13" s="14">
         <v>44256</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="15" customHeight="1">
+      <c r="A14" s="25" t="s">
+        <v>256</v>
+      </c>
+      <c r="B14" s="2">
+        <v>11</v>
+      </c>
+      <c r="C14" s="36">
+        <v>44317</v>
+      </c>
+      <c r="D14" s="2">
+        <v>1</v>
+      </c>
+      <c r="E14" s="36">
+        <v>44317</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add check overlap for same offering.
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apple/cs2102-team61/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD8486ED-772B-2F44-AA9B-69CA3F4E235D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC34EB2D-2C76-2B4E-9572-EB7A67CFB798}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="9" activeTab="22" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Employees" sheetId="1" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="286">
   <si>
     <t>eid</t>
   </si>
@@ -905,6 +905,15 @@
   </si>
   <si>
     <t>easy AI module</t>
+  </si>
+  <si>
+    <t>Zoe Wang</t>
+  </si>
+  <si>
+    <t>zoe@gmail.com</t>
+  </si>
+  <si>
+    <t>(+65) 10103399</t>
   </si>
 </sst>
 </file>
@@ -915,7 +924,7 @@
     <numFmt numFmtId="164" formatCode="yyyy\-mm\-dd"/>
     <numFmt numFmtId="165" formatCode="yyyy\-m\-d"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -955,6 +964,12 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="6">
@@ -1005,10 +1020,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -1066,8 +1082,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1284,10 +1302,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:G21"/>
+  <dimension ref="A1:G22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G8" sqref="G8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -1738,7 +1756,30 @@
         <v>44295</v>
       </c>
     </row>
+    <row r="22" spans="1:7" ht="15" customHeight="1">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>284</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="F22" s="5">
+        <v>43134</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="C22" r:id="rId1" xr:uid="{F9A9486A-83A1-6448-9FC6-92475FC6954C}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
@@ -2029,7 +2070,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E10" sqref="E10"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2137,10 +2178,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -2260,6 +2301,14 @@
       </c>
       <c r="B14" s="8" t="s">
         <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" customHeight="1">
+      <c r="A15" s="2">
+        <v>21</v>
+      </c>
+      <c r="B15" s="10" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -3108,7 +3157,7 @@
   <dimension ref="A1:H41"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H41" sqref="H41"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -5467,10 +5516,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:B14"/>
+  <dimension ref="A1:B15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -5588,6 +5637,14 @@
       </c>
       <c r="B14" s="4">
         <v>1790</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" ht="15" customHeight="1">
+      <c r="A15" s="2">
+        <v>21</v>
+      </c>
+      <c r="B15" s="2">
+        <v>1500</v>
       </c>
     </row>
   </sheetData>
@@ -6371,7 +6428,7 @@
   </sheetPr>
   <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -6592,10 +6649,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A14"/>
+  <dimension ref="A1:A15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD1048576"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -6671,6 +6728,11 @@
     <row r="14" spans="1:1" ht="15.75" customHeight="1">
       <c r="A14" s="4">
         <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" ht="15" customHeight="1">
+      <c r="A15" s="2">
+        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -6684,10 +6746,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:A7"/>
+  <dimension ref="A1:A8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD1048576"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1"/>
@@ -6728,6 +6790,11 @@
     <row r="7" spans="1:1" ht="15.75" customHeight="1">
       <c r="A7" s="4">
         <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" ht="15" customHeight="1">
+      <c r="A8" s="2">
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>